<commit_message>
Updated definition of sameple and template dataset
</commit_message>
<xml_diff>
--- a/web_prototype/DataTemplate.xlsx
+++ b/web_prototype/DataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eason\Desktop\Y4S1\FIT3164\ZPrototype\FIT3164_software\web3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiaxin/Desktop/FIT3164/FIT3164_software/web_prototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280450D3-E425-4651-991A-B66E0CC6C34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB9842C-57BA-9849-AE7E-446946A899D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTemplate" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -244,14 +244,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,6 +935,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-MY" sz="1200" b="1" i="0">
               <a:solidFill>
@@ -970,20 +986,148 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>recon - Breast Reconstruction</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>recon - Breast Reconstruction. '0'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> means no reconstruction, '1' means </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TRAM flap, '2' means implant</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-MY" sz="1200" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-MY" sz="1200" b="1"/>
             <a:t>25.</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-MY" sz="1200" baseline="0"/>
-            <a:t> tax - Taxane-based Chemotherapy</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t> tax - Taxane-based Chemotherapy.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'0'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> means no taxane, '1' means type 1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, '2' means type 2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-MY" sz="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-MY" sz="1200" b="1" baseline="0"/>
             <a:t>26.</a:t>
@@ -1002,10 +1146,48 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>che - Chemotherapy</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>che - Chemotherapy. '0'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> means no, '1' means yes.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-MY" sz="1200" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-MY" sz="1200" b="1" i="0">
               <a:solidFill>
@@ -1028,8 +1210,29 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> axi - Axilla Radiation Therapy</a:t>
-          </a:r>
+            <a:t> axi - Axilla Radiation Therapy. '0'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> means no, '1' means yes.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-MY" sz="1200" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -1377,19 +1580,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="31" max="31" width="39.7109375" customWidth="1"/>
-    <col min="32" max="32" width="36.5703125" customWidth="1"/>
+    <col min="31" max="31" width="39.6640625" customWidth="1"/>
+    <col min="32" max="32" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1579,33 +1782,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="AE11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1616,11 +1816,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3699753-688F-4C76-BDF6-5B9D30F03E0C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
uploading all final dataset files
</commit_message>
<xml_diff>
--- a/web_prototype/DataTemplate.xlsx
+++ b/web_prototype/DataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIT3164_software\web_prototype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eason\Desktop\Y4S1\FIT3164\ZPrototype\FIT3164_software\web3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625D001C-6E57-4A6A-9B97-B03A17BC77FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A860CF92-E763-4962-A336-2010A6A7B3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTemplate" sheetId="1" r:id="rId1"/>
@@ -270,22 +270,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
+        <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FE298B5-D564-47EF-B46E-1BFA6B91F74B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58897878-3E03-4194-B257-6ABE7C8F8C9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -293,8 +293,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="619125" y="200025"/>
-          <a:ext cx="6705600" cy="5895975"/>
+          <a:off x="590550" y="190500"/>
+          <a:ext cx="6696075" cy="5715000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -329,7 +329,9 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-MY" sz="1400" b="1"/>
+            <a:rPr lang="en-MY" sz="1400" b="1">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>Definition of features/columns:</a:t>
           </a:r>
         </a:p>
@@ -340,7 +342,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -352,7 +354,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -366,7 +368,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -378,7 +380,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -392,7 +394,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -404,7 +406,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -418,7 +420,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -430,7 +432,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -444,7 +446,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -456,7 +458,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -470,7 +472,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -482,7 +484,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -496,7 +498,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -508,7 +510,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -522,7 +524,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -534,7 +536,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -548,7 +550,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -560,7 +562,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -574,7 +576,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -586,7 +588,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -600,7 +602,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -612,7 +614,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -626,7 +628,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -638,7 +640,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -652,7 +654,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -664,7 +666,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -678,7 +680,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -690,7 +692,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -704,7 +706,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -716,7 +718,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -730,7 +732,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -742,7 +744,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -756,7 +758,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -768,7 +770,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -782,7 +784,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -794,7 +796,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -808,7 +810,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -820,7 +822,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -834,7 +836,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -846,7 +848,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -860,7 +862,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -872,7 +874,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -886,7 +888,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -898,7 +900,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -912,7 +914,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -924,7 +926,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -955,7 +957,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -967,7 +969,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -979,7 +981,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -991,7 +993,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1003,7 +1005,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1015,7 +1017,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1026,7 +1028,7 @@
               <a:schemeClr val="dk1"/>
             </a:solidFill>
             <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
@@ -1050,11 +1052,15 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-MY" sz="1200" b="1"/>
+            <a:rPr lang="en-MY" sz="1200" b="1">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>25.</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-MY" sz="1200" baseline="0"/>
+            <a:rPr lang="en-MY" sz="1200" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t> tax - Taxane-based Chemotherapy.  </a:t>
           </a:r>
           <a:r>
@@ -1063,7 +1069,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1075,7 +1081,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1087,7 +1093,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1099,13 +1105,15 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-MY" sz="1200" baseline="0"/>
+          <a:endParaRPr lang="en-MY" sz="1200" baseline="0">
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -1126,11 +1134,15 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-MY" sz="1200" b="1" baseline="0"/>
+            <a:rPr lang="en-MY" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>26.</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-MY" sz="1200" baseline="0"/>
+            <a:rPr lang="en-MY" sz="1200" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
@@ -1139,7 +1151,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1151,7 +1163,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1162,7 +1174,7 @@
               <a:schemeClr val="dk1"/>
             </a:solidFill>
             <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
@@ -1191,7 +1203,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1203,7 +1215,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1215,7 +1227,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1226,7 +1238,7 @@
               <a:schemeClr val="dk1"/>
             </a:solidFill>
             <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
@@ -1238,7 +1250,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -1250,62 +1262,12 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t> Hb - Hemoglobin</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1200" b="1" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>29.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1200" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Endpoint - The dependent variable. '0'</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1200" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> means lymphedema absent, '1' means lymphedema present.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-MY" sz="1200" b="0" i="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-MY" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1579,17 +1541,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="30" max="30" width="39.6328125" customWidth="1"/>
-    <col min="31" max="31" width="36.453125" customWidth="1"/>
+    <col min="30" max="30" width="39.5703125" customWidth="1"/>
+    <col min="31" max="31" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1678,7 +1640,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -1773,27 +1735,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1807,11 +1769,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3699753-688F-4C76-BDF6-5B9D30F03E0C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>